<commit_message>
issue 209: get tests green again
</commit_message>
<xml_diff>
--- a/jxls-poi/src/test/resources/org/jxls/templatebasedtests/Issue209Test_old.xlsx
+++ b/jxls-poi/src/test/resources/org/jxls/templatebasedtests/Issue209Test_old.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\2023Stuff\GitRepos\jxls\jxls-poi\src\test\resources\org\jxls\templatebasedtests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA019378-A4FA-45F6-A337-2A3AF60732E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BF79A2-03C6-428A-9D0C-6C5D439BB6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{FD9617C2-E059-4346-A6DF-EED55EE48DC3}"/>
   </bookViews>
@@ -84,7 +84,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="employees" var="d" groupBy="department" groupOrder="ASC" select="d.item.department=='Department A'" lastCell="H5")</t>
+jx:each(items="employees" var="d" groupBy="department" groupOrder="ASC" select="d.item.department=='Department A'" lastCell="H5" oldSelectBehavior="true")</t>
         </r>
       </text>
     </comment>

</xml_diff>